<commit_message>
work on facility corrections for Fedex and USPS
</commit_message>
<xml_diff>
--- a/YellowstonePathology/TestingDialog.xlsx
+++ b/YellowstonePathology/TestingDialog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Histology Slide ZPL" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="81">
   <si>
     <t>Testing the edges of the truncation:</t>
   </si>
@@ -211,7 +211,73 @@
     <t xml:space="preserve">check to make sure that cases are added to this list when the case is created. </t>
   </si>
   <si>
-    <t xml:space="preserve">Why was the needs gross box not checked on test specimen/patient </t>
+    <t xml:space="preserve">Why was the "needs gross" box not checked on test specimen/patient </t>
+  </si>
+  <si>
+    <t>Checked the Not Scanned List.</t>
+  </si>
+  <si>
+    <t>Noted that some client accessioned cases were showing up on the list.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These cases show up because the block was not checekd as client accessioned at accessioning. </t>
+  </si>
+  <si>
+    <t>It will be communicated to accessioning staff that all client accessioned cases must hae the blocks marked as client accessioned to keep these cases from the Not Scanned List.</t>
+  </si>
+  <si>
+    <t>Test to see if putting one block on hold works</t>
+  </si>
+  <si>
+    <t>Test to see if putting an entire case on hold works</t>
+  </si>
+  <si>
+    <t>A MM case is created with mulitiple blocks, taken to the gross station and the whole case is put on hold</t>
+  </si>
+  <si>
+    <t>A MM case is created with mulitiple blocks, taken to the gross station and one block is put on hold. Press and hold the block you want and select the hold block option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test embedding dialog setting fixation time. </t>
+  </si>
+  <si>
+    <t>scan a block from yesterday and see if it sets the fixation time with an additional 24 hrs.</t>
+  </si>
+  <si>
+    <t>scan  a block from yesterday that has been incorrectly set and properly set the fixation time from the embedding dialog</t>
+  </si>
+  <si>
+    <t>scan a block from several days ago and see if the fixation time is reset to an incorrect value.</t>
+  </si>
+  <si>
+    <t>Scan a MM case created today to make sure that the fixation duration is still setting correctly for a specimen that has not been previously scanned.</t>
+  </si>
+  <si>
+    <t>Scan a case from two days ago to see if fixation duration is updated.</t>
+  </si>
+  <si>
+    <t>while setting fixation time worked fine there was the error that allows for negative fixation duration.</t>
+  </si>
+  <si>
+    <t>Sid to fix.</t>
+  </si>
+  <si>
+    <t>When dealing with client accession cases the end time/ fixation duration isn't noted on the Breast Case list in the embedding dialog.</t>
+  </si>
+  <si>
+    <t>Sid to deal with.</t>
+  </si>
+  <si>
+    <t>10/17/2016 … corrected/ annotated following discussion with Sid 10/18/2016</t>
+  </si>
+  <si>
+    <t>Check to verify that the fixation duration being listed is also the duration that was entered via the mapping page.</t>
+  </si>
+  <si>
+    <t>Look at the fixation duration in the embedding diolog and compare the number there to the number entered in the mapping for client accessioned cases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is a rounding error that ends with the duration being an hour off one way or the other. There are "0" durations. </t>
   </si>
 </sst>
 </file>
@@ -688,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -788,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +863,7 @@
     <col min="1" max="1" width="18.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.875" style="1" customWidth="1"/>
     <col min="3" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" style="1" customWidth="1"/>
     <col min="6" max="6" width="1.375" style="19" customWidth="1"/>
     <col min="7" max="7" width="17.875" style="7" customWidth="1"/>
     <col min="8" max="10" width="18.125" style="1" customWidth="1"/>
@@ -1002,13 +1068,13 @@
         <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="25">
-        <v>42660</v>
+        <v>76</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>77</v>
       </c>
       <c r="G6" s="24" t="s">
         <v>55</v>
@@ -1069,6 +1135,24 @@
       <c r="J7" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K7" s="25">
+        <v>42660</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q7" s="25">
+        <v>42661</v>
+      </c>
     </row>
     <row r="8" spans="1:17" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1086,11 +1170,126 @@
       <c r="E8" s="25">
         <v>42660</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="25">
+        <v>42661</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="25">
+        <v>42661</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="25">
+        <v>42661</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="25">
+        <v>42661</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="25">
+        <v>42661</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="25">
+        <v>42661</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q11" s="25">
+        <v>42661</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="13" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
documentation for lynch syndrom in testingdialog
</commit_message>
<xml_diff>
--- a/YellowstonePathology/TestingDialog.xlsx
+++ b/YellowstonePathology/TestingDialog.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Histology Slide ZPL" sheetId="1" r:id="rId1"/>
+    <sheet name="Histology ZPL" sheetId="1" r:id="rId1"/>
     <sheet name="Embedding Dialog" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Random Testing" sheetId="3" r:id="rId3"/>
+    <sheet name="Lynch Syndrome" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="142">
   <si>
     <t>Testing the edges of the truncation:</t>
   </si>
@@ -288,12 +289,186 @@
   <si>
     <t>all labels look appropriate</t>
   </si>
+  <si>
+    <t>Test to verify that the Slide Label and the Block Label scan at all locations</t>
+  </si>
+  <si>
+    <t>print a MM paper label for blocvk and slide and test their scanning capability at the cutting station, the material tracting, and at the pathologist work areas.</t>
+  </si>
+  <si>
+    <t>slide labels did not scan in material tracking.</t>
+  </si>
+  <si>
+    <t>Sent to Sid for remedy. Computers didn't have to correct code; restart the computer fixed the problem.</t>
+  </si>
+  <si>
+    <t>Test to see if when adding blocks to a case the system errors and mis-creates the blocks.</t>
+  </si>
+  <si>
+    <t>Create a block on a MM case. Then after saving, refreshing, go back in to the case and add another another block save refresh and go back in again.</t>
+  </si>
+  <si>
+    <t>worked fine block stayed labeled correctly</t>
+  </si>
+  <si>
+    <t>Try and figure out why occasionally the client supply order ends up blank after it has been filled.</t>
+  </si>
+  <si>
+    <t>Create multiple client supply orders to see if any fail to stay filled</t>
+  </si>
+  <si>
+    <t>all supply orders entered worked fine</t>
+  </si>
+  <si>
+    <t>Mutation</t>
+  </si>
+  <si>
+    <t>Intact</t>
+  </si>
+  <si>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>MLH1</t>
+  </si>
+  <si>
+    <t>MLH2</t>
+  </si>
+  <si>
+    <t>MLH6</t>
+  </si>
+  <si>
+    <t>PMS2</t>
+  </si>
+  <si>
+    <t>BRAF</t>
+  </si>
+  <si>
+    <t>Meth</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>all Intact</t>
+  </si>
+  <si>
+    <t>only MLH1  lost</t>
+  </si>
+  <si>
+    <t>MLH1 &amp; 2 lost</t>
+  </si>
+  <si>
+    <t>MLH1, 2, &amp; 6 lost</t>
+  </si>
+  <si>
+    <t>All Lost</t>
+  </si>
+  <si>
+    <t>only PMS2 lost</t>
+  </si>
+  <si>
+    <t>PMS2 &amp; MLH6 lost</t>
+  </si>
+  <si>
+    <t>PMS2, MLH6, and MLH2 lost</t>
+  </si>
+  <si>
+    <t>Interpretation</t>
+  </si>
+  <si>
+    <t>only MLH2 lost</t>
+  </si>
+  <si>
+    <t>only MLH6 lost</t>
+  </si>
+  <si>
+    <t>MLH2 &amp; PMS2 lost</t>
+  </si>
+  <si>
+    <t>MLH1 &amp; MLH6 lost</t>
+  </si>
+  <si>
+    <t>Gentetics</t>
+  </si>
+  <si>
+    <t>MLH2 &amp; 6 lost</t>
+  </si>
+  <si>
+    <t>needs done</t>
+  </si>
+  <si>
+    <t>Current  Model</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>No loss of Expression</t>
+  </si>
+  <si>
+    <t>Loss of Nuclear expression of MLH1 and PMS2</t>
+  </si>
+  <si>
+    <t>Loss of Nuclear expression of MSH2 and MSH6</t>
+  </si>
+  <si>
+    <t>Loss of Nuclear expression of MLH1 only</t>
+  </si>
+  <si>
+    <t>Loss of Nuclear expression of MSH6 only</t>
+  </si>
+  <si>
+    <t>Loss of Nuclear expression of PMS2 only</t>
+  </si>
+  <si>
+    <t>All results are set to Intact expression on the IHC results page. The evaluation page has the 4 mutation options set to "positive" and BRAF/Meth set to "not applicable". Order Status: LSECOLON says "No further testing is required"; LSEGYN is blank.</t>
+  </si>
+  <si>
+    <t>results are set properly on the IHC page with MLH1 and PMS2 being set to loss of expression and the remaining 2 set to intact. Evaluation page has MLH1 and PMS2 set to "negative" and the reamining 2 to "positive". Order status: LSECOLON says BRAF testing is required and should be ordered; LSEGYN says Methylation Analysis Testing is required and should be ordered. Upon ordering the BRAF the Order status changes to "and has been ordered". BRAF is positive no further testing. BRAF negative comment changes to "Methylation Analysis testing is required and should be ordered" upon ordering BRAF and Meth a pop-up shows up saying the case would benefit from a Comprehensive Colon Cancer profile.</t>
+  </si>
+  <si>
+    <t>results are set correctly on IHC page. Results are set correctly on the Evaluation page. Order status: LSECOLON says no further testing required; LSEGYN is blank.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results set correctly on IHC. Set correctly on the Evaluation page. Order status: LSECOLON says a BRAF should be ordered; LSEGYN says a Methylation Analysis test should be ordered. BRAF Neg comment simply says it has been ordered, nothing about needing Methylation Analysis. </t>
+  </si>
+  <si>
+    <t>Restuls are set correctly on IHC page and the Evaluation page. The order status says No furhter testing required for LSECOLON and is blank for LSEGYN.</t>
+  </si>
+  <si>
+    <t>Results are set correctly on the IHC and Evaluation pages. Order status says no further testin gon LSECOLON and is blank on the LSEGYN.</t>
+  </si>
+  <si>
+    <t>New Model</t>
+  </si>
+  <si>
+    <t>Intact on the IHC result page correlates to intact on the Evaluation result page. Order status says no further testing for LSECOLO and is blank for LSEGYN</t>
+  </si>
+  <si>
+    <t>Intact/Loss correlates between IHC results and Evaluation results pages. Order status LSECOLON says no further testing required and is blank for LSEGYN</t>
+  </si>
+  <si>
+    <t>Intact/Loss results correlate. Status LSECOLON no further testing required, LSEGYN blank</t>
+  </si>
+  <si>
+    <t>intact/loss results correlate. LSECOLON no further testing, LSEGYN blank.</t>
+  </si>
+  <si>
+    <t>Intact/loss correlates. Order status LSECOLO requests BRAF, LSEGYN is blank. LSECOLON status changes to BRAF has been ordered. LSEGYN has no comment. BRAF positive and negative result In the order status staying at BRAF required and has been ordered. No request for Methylation analysis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intact/Loss correlates from IHC to Evaluation. Order status for LSECOLO requests BRAF be ordered, LSE GYN is blank. Status comments that the BRAF has been ordered. LSEGYN has no comment. BRAF positive nothing changes, BRAF Negative Order status changes to say Methylation Analysis testing is required. Ordering the Meth results in the Order status changing to say simply that the Meth analysis has been ordered. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,8 +507,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,6 +552,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -383,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -458,6 +652,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -763,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +1055,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:4" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="8" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1327,12 +1540,640 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="25.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="21"/>
+      <c r="B1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="21"/>
+      <c r="H4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" s="21"/>
+      <c r="H14" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="21"/>
+      <c r="H16" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="21"/>
+      <c r="H17" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="393" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="188.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="21"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="21"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changes to twin placenta template and addition of Bladder TUR
</commit_message>
<xml_diff>
--- a/YellowstonePathology/TestingDialog.xlsx
+++ b/YellowstonePathology/TestingDialog.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Histology ZPL" sheetId="1" r:id="rId1"/>
     <sheet name="Embedding Dialog" sheetId="2" r:id="rId2"/>
     <sheet name="Random Testing" sheetId="3" r:id="rId3"/>
     <sheet name="Lynch Syndrome" sheetId="4" r:id="rId4"/>
+    <sheet name="EGFR ALK ROS1 testing" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="156">
   <si>
     <t>Testing the edges of the truncation:</t>
   </si>
@@ -458,9 +459,6 @@
     <t>intact/loss results correlate. LSECOLON no further testing, LSEGYN blank.</t>
   </si>
   <si>
-    <t>Intact/loss correlates. Order status LSECOLO requests BRAF, LSEGYN is blank. LSECOLON status changes to BRAF has been ordered. LSEGYN has no comment. BRAF positive and negative result In the order status staying at BRAF required and has been ordered. No request for Methylation analysis.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Intact/Loss correlates from IHC to Evaluation. Order status for LSECOLO requests BRAF be ordered, LSE GYN is blank. Status comments that the BRAF has been ordered. LSEGYN has no comment. BRAF positive nothing changes, BRAF Negative Order status changes to say Methylation Analysis testing is required. Ordering the Meth results in the Order status changing to say simply that the Meth analysis has been ordered. </t>
   </si>
   <si>
@@ -471,6 +469,42 @@
   </si>
   <si>
     <t>worked fine scanned at both locations</t>
+  </si>
+  <si>
+    <t>create a MM case for each possible option in the system and check how they result all the way to the end of the process; ending with finalizing the case itself</t>
+  </si>
+  <si>
+    <t>loss of MSH6 and PMS2</t>
+  </si>
+  <si>
+    <t>no way for this option to be chosen.</t>
+  </si>
+  <si>
+    <t>requested BRAF order but with a negative BRAF a MethA should be requested and it isnt. Thus you cant set the results as it doesn’t match a defined set</t>
+  </si>
+  <si>
+    <t>Intact/loss correlates. Order status LSECOLO requests BRAF, LSEGYN is blank. LSECOLON status changes to BRAF has been ordered. LSEGYN has no comment. BRAF positive and negative result In the order status staying at BRAF required and has been ordered. **No request for Methylation analysis.**</t>
+  </si>
+  <si>
+    <t>test to see how the changes to the PDL-1 and EGFR ALK ROS-1 reflex group are working</t>
+  </si>
+  <si>
+    <t>created a MM case and ordered a surgical. From the Pathology Workspace a EGFR, ALK, ROS-1 reflex analysis was ordered. The reflex tests will be resulted and analyzed to see the outcomes and how everything interacts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> for a non pathology associates affiliate the ordering of the EGFR ALK ROS1 and PDL -1 was ordered and resulted as expected per assistance by Sean Gratwold.</t>
+  </si>
+  <si>
+    <t>for a pathology associates MM case all results worked as expected</t>
+  </si>
+  <si>
+    <t>please note there was the odd occurance where it said the results could not be accepted as they were already accepted.</t>
+  </si>
+  <si>
+    <t>if LSEGYN is chosen the "order status" doesn't give any information on what might need to be ordered. When set to LSECOLON results cannot be set…the message "Restuls cnnot be set because results do not match a defines set".</t>
+  </si>
+  <si>
+    <t>what was done</t>
   </si>
 </sst>
 </file>
@@ -972,19 +1006,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" style="1" customWidth="1"/>
     <col min="3" max="4" width="36" style="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1080,13 +1114,13 @@
     </row>
     <row r="8" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
@@ -1113,21 +1147,21 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
     <col min="3" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="1.375" style="19" customWidth="1"/>
-    <col min="7" max="7" width="17.875" style="7" customWidth="1"/>
-    <col min="8" max="10" width="18.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="1.125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="1.42578125" style="19" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="7" customWidth="1"/>
+    <col min="8" max="10" width="18.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="1.140625" style="21" customWidth="1"/>
     <col min="13" max="13" width="18" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" style="1" customWidth="1"/>
     <col min="15" max="16" width="18" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.25" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" style="1" customWidth="1"/>
     <col min="18" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1568,11 +1602,11 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
@@ -1634,23 +1668,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="25.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="18" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -2134,13 +2168,13 @@
         <v>136</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>137</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>138</v>
@@ -2157,45 +2191,114 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="H31" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update to testing dialog
</commit_message>
<xml_diff>
--- a/YellowstonePathology/TestingDialog.xlsx
+++ b/YellowstonePathology/TestingDialog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Histology ZPL" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="166">
   <si>
     <t>Testing the edges of the truncation:</t>
   </si>
@@ -505,6 +505,36 @@
   </si>
   <si>
     <t>what was done</t>
+  </si>
+  <si>
+    <t>Test to see is the assignment page comes up on IHC QC and Informal Consults</t>
+  </si>
+  <si>
+    <t>Create a MM case with an IHC, and one with an Informal Consult and proceed to where the assignment page should be.</t>
+  </si>
+  <si>
+    <t>One worked one did not</t>
+  </si>
+  <si>
+    <t>Sid was notified and said he would fix the problem.</t>
+  </si>
+  <si>
+    <t>Test the added Bladder TUR template to make sure that the Block submission code works properly.</t>
+  </si>
+  <si>
+    <t>create a MM case with a Bladder TUR template and multiple blocks</t>
+  </si>
+  <si>
+    <t>Everything worked correctly</t>
+  </si>
+  <si>
+    <t>create multiple MM cases with each of the special characters in question and one or two with no spaces or anything like is normal now and see if the linking page finds all of the patient cases to be linked.</t>
+  </si>
+  <si>
+    <t>Check to see how linking works with hyphens(-), apostrophies('), and spaces in the patient name and with multiple letters in the middle initial space</t>
+  </si>
+  <si>
+    <t>works as Sid expected it to</t>
   </si>
 </sst>
 </file>
@@ -1596,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1659,6 +1689,48 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1668,7 +1740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
addition of fallopian tubes with ovaries template
</commit_message>
<xml_diff>
--- a/YellowstonePathology/TestingDialog.xlsx
+++ b/YellowstonePathology/TestingDialog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Histology ZPL" sheetId="1" r:id="rId1"/>
@@ -1628,7 +1628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1740,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2234,7 +2234,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="188.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="240.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="1" t="s">
         <v>136</v>

</xml_diff>